<commit_message>
Added calculation for 3.3v and 12v buck converters.
</commit_message>
<xml_diff>
--- a/doc/LM3150MHX Calculator.xlsx
+++ b/doc/LM3150MHX Calculator.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\SAS-Backplane\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DCDC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38362D9-F28C-45E0-9F8E-554664943721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7208DA5-29C5-4DC1-8B34-324C95A8E329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="530" yWindow="0" windowWidth="17320" windowHeight="19950" xr2:uid="{C17DE87D-D3A8-4F0B-998C-A262C791429E}"/>
+    <workbookView xWindow="530" yWindow="0" windowWidth="17320" windowHeight="19950" activeTab="1" xr2:uid="{C17DE87D-D3A8-4F0B-998C-A262C791429E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Calculation" sheetId="1" r:id="rId1"/>
+    <sheet name="5V" sheetId="1" r:id="rId1"/>
+    <sheet name="3.3V" sheetId="2" r:id="rId2"/>
+    <sheet name="12V" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="82">
   <si>
     <t>LM3150MHX/NOPB Calculator</t>
   </si>
@@ -340,7 +342,147 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -428,23 +570,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>711011</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>2893</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>53882</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 2">
+        <xdr:cNvPr id="4" name="Grafik 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFCED43C-7AAE-4E38-AF44-4E41B21338BE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBF752B4-A587-4329-8B5A-839D55E31321}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -460,8 +602,106 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4025711" y="200026"/>
-          <a:ext cx="5616482" cy="2695574"/>
+          <a:off x="4051300" y="184150"/>
+          <a:ext cx="5387882" cy="2743199"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>53882</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C219DBCD-5B0A-4997-97EE-DE56E97C974D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4051300" y="184150"/>
+          <a:ext cx="5387882" cy="2743199"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>53882</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC2CEE49-F19B-4EA2-A0E9-A088FAA54CE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4051300" y="184150"/>
+          <a:ext cx="5387882" cy="2743199"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -772,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C0D372-FD9A-401D-80C0-F303A26CDA15}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -953,15 +1193,15 @@
         <v>23</v>
       </c>
       <c r="F18" s="1">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="G18">
         <f>B18-B18*F18</f>
-        <v>72600.000000000015</v>
+        <v>71866.666666666672</v>
       </c>
       <c r="H18">
         <f>B18+B18*F18</f>
-        <v>74066.666666666672</v>
+        <v>74800.000000000015</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1585,18 +1825,1728 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="lessThan">
       <formula>$E$28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="greaterThan">
       <formula>$F$28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="lessThan">
       <formula>$G$18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="greaterThan">
+      <formula>$H$18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B56">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
+      <formula>$B$57</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B64">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
+      <formula>$B$57</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
+      <formula>$B$7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{E45BFA85-D7EA-4DEE-928D-EE60C8A55F03}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDCA830-8D2C-4258-99A0-6269838FD908}">
+  <dimension ref="A1:H74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:XFD65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4">
+        <f>0.000005</f>
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13">
+        <f>B13*1000*1000</f>
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="4">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14">
+        <f>B14/100</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="4">
+        <f>10000+330</f>
+        <v>10330</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <f>B17/1000</f>
+        <v>10.33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <f>B17*(B7/B4-1)</f>
+        <v>46485</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <f>B18/1000</f>
+        <v>46.484999999999999</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G18">
+        <f>B18-B18*F18</f>
+        <v>45555.3</v>
+      </c>
+      <c r="H18">
+        <f>B18+B18*F18</f>
+        <v>47414.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="4">
+        <v>47000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19">
+        <f>B19/1000</f>
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="5">
+        <f>(B19/B17+1)*B4</f>
+        <v>3.329912875121007</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <f>B7/B10</f>
+        <v>0.20624999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24">
+        <f>B7/B9</f>
+        <v>0.27499999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <f>B7/B8</f>
+        <v>0.54999999999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <f>B23/(0.0000002)</f>
+        <v>1031250</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <f>(1-B25)/B26</f>
+        <v>4.3636363636363641E-7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27">
+        <f>B27*10000000</f>
+        <v>4.3636363636363642</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <f>(1-B25)/(B27+0.0000002)</f>
+        <v>707142.85714285716</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E28">
+        <f>B28-B28*D28</f>
+        <v>636428.57142857148</v>
+      </c>
+      <c r="F28">
+        <f>B28+B28*D28</f>
+        <v>777857.14285714284</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4">
+        <v>700000</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29">
+        <f>B29/1000</f>
+        <v>700</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f>-((B9-1)*(B9*16.5+100))-1000</f>
+        <v>-4278</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30">
+        <f>B30/1000</f>
+        <v>-4.2779999999999996</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <f>((B7*B9)-B7)/(B9*0.0000000001*B29)+(B30)</f>
+        <v>38936.28571428571</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="5">
+        <f>B31/1000</f>
+        <v>38.93628571428571</v>
+      </c>
+      <c r="E31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34">
+        <f>(B10-B7)*(B7/B10)*(1/B29)</f>
+        <v>3.7419642857142854E-6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34">
+        <f>B34*1000000</f>
+        <v>3.7419642857142854</v>
+      </c>
+      <c r="E34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37">
+        <f>B9*0.3/12^(1/2)</f>
+        <v>1.0392304845413263</v>
+      </c>
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E37">
+        <f>B37-B37*D37</f>
+        <v>0.98726896031425992</v>
+      </c>
+      <c r="F37">
+        <f>B37+B37*D37</f>
+        <v>1.0911920087683926</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38">
+        <f>(B7/B9)/B29</f>
+        <v>3.9285714285714281E-7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38">
+        <f>B38*1000000000</f>
+        <v>392.85714285714283</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39">
+        <f>70/(B29^2*0.00000165)</f>
+        <v>8.658008658008658E-5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="5">
+        <f>B39*1000000</f>
+        <v>86.580086580086586</v>
+      </c>
+      <c r="E39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <f>(0.08*B39*B37*1)/B34</f>
+        <v>1.9236242456243144</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40">
+        <f>B40*1000</f>
+        <v>1923.6242456243144</v>
+      </c>
+      <c r="E40" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <f>(B7/(B8*B29))*((B17+B19)/(B17*B19))</f>
+        <v>9.2778727523634948E-11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="5">
+        <f>B44*1000000000000</f>
+        <v>92.778727523634942</v>
+      </c>
+      <c r="E44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47">
+        <f>1.2*B10</f>
+        <v>19.2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" s="4">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="4">
+        <v>150</v>
+      </c>
+      <c r="C52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="4">
+        <v>30</v>
+      </c>
+      <c r="C53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54">
+        <f>B11^2*B49*B24</f>
+        <v>0.21999999999999997</v>
+      </c>
+      <c r="C54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f>0.5*B9*B11*0.0000000015*B29*(8.5/(B50-B51)+6.8/B51)</f>
+        <v>0.38945454545454544</v>
+      </c>
+      <c r="C55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56">
+        <f>B54+B55</f>
+        <v>0.60945454545454547</v>
+      </c>
+      <c r="C56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57">
+        <f>B52/B53</f>
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" s="4">
+        <f>B49</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" s="4">
+        <f>B50</f>
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" s="4">
+        <f>B51</f>
+        <v>1.6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" s="4">
+        <f>B52</f>
+        <v>150</v>
+      </c>
+      <c r="C62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" s="4">
+        <f>B53</f>
+        <v>30</v>
+      </c>
+      <c r="C63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64">
+        <f>B11^2*B59*(1-B24)</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="C64" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68">
+        <f>D14*B9</f>
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69">
+        <f>(B11*B24*(1-B24))/(B29*B68)</f>
+        <v>4.7470238095238085E-6</v>
+      </c>
+      <c r="C69" t="s">
+        <v>43</v>
+      </c>
+      <c r="D69" s="5">
+        <f>B69*1000000</f>
+        <v>4.7470238095238084</v>
+      </c>
+      <c r="E69" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72">
+        <v>0.6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="3">
+        <v>7.7000000000000008E-6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73">
+        <f>B73*1000000</f>
+        <v>7.7000000000000011</v>
+      </c>
+      <c r="E73" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74">
+        <f>-(B73*B13)/B72</f>
+        <v>-6.4166666666666691E-11</v>
+      </c>
+      <c r="C74" t="s">
+        <v>43</v>
+      </c>
+      <c r="D74">
+        <f>B74*1000000</f>
+        <v>-6.416666666666669E-5</v>
+      </c>
+      <c r="E74" t="s">
+        <v>36</v>
+      </c>
+      <c r="F74" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
+      <formula>$E$28</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="greaterThan">
+      <formula>$F$28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="lessThan">
+      <formula>$G$18</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="greaterThan">
+      <formula>$H$18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B56">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+      <formula>$B$57</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B64">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+      <formula>$B$57</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+      <formula>$B$7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{27002FD1-C7D4-4B84-9FEB-22EF75521F33}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18A6C88-0247-4D30-92B5-0F853FB0062C}">
+  <dimension ref="A1:H74"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4">
+        <f>0.000005</f>
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13">
+        <f>B13*1000*1000</f>
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="4">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14">
+        <f>B14/100</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="4">
+        <f>10000+330</f>
+        <v>10330</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <f>B17/1000</f>
+        <v>10.33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <f>B17*(B7/B4-1)</f>
+        <v>196270</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <f>B18/1000</f>
+        <v>196.27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G18">
+        <f>B18-B18*F18</f>
+        <v>192344.6</v>
+      </c>
+      <c r="H18">
+        <f>B18+B18*F18</f>
+        <v>200195.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="4">
+        <v>200000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19">
+        <f>B19/1000</f>
+        <v>200</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="5">
+        <f>(B19/B17+1)*B4</f>
+        <v>12.216650532429815</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <f>B7/B10</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24">
+        <f>B7/B9</f>
+        <v>0.70588235294117652</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <f>B7/B8</f>
+        <v>0.8571428571428571</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <f>B23/(0.0000002)</f>
+        <v>2500000</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <f>(1-B25)/B26</f>
+        <v>5.7142857142857164E-8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27">
+        <f>B27*10000000</f>
+        <v>0.57142857142857162</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <f>(1-B25)/(B27+0.0000002)</f>
+        <v>555555.55555555574</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E28">
+        <f>B28-B28*D28</f>
+        <v>500000.00000000017</v>
+      </c>
+      <c r="F28">
+        <f>B28+B28*D28</f>
+        <v>611111.11111111136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4">
+        <v>550000</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29">
+        <f>B29/1000</f>
+        <v>550</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f>-((B9-1)*(B9*16.5+100))-1000</f>
+        <v>-7088</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30">
+        <f>B30/1000</f>
+        <v>-7.0880000000000001</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <f>((B7*B9)-B7)/(B9*0.0000000001*B29)+(B30)</f>
+        <v>198259.5935828877</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="5">
+        <f>B31/1000</f>
+        <v>198.2595935828877</v>
+      </c>
+      <c r="E31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34">
+        <f>(B10-B7)*(B7/B10)*(1/B29)</f>
+        <v>1.0909090909090909E-5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34">
+        <f>B34*1000000</f>
+        <v>10.909090909090908</v>
+      </c>
+      <c r="E34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37">
+        <f>B9*0.3/12^(1/2)</f>
+        <v>1.4722431864335457</v>
+      </c>
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E37">
+        <f>B37-B37*D37</f>
+        <v>1.3986310271118685</v>
+      </c>
+      <c r="F37">
+        <f>B37+B37*D37</f>
+        <v>1.5458553457552229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38">
+        <f>(B7/B9)/B29</f>
+        <v>1.2834224598930481E-6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38">
+        <f>B38*1000000000</f>
+        <v>1283.4224598930482</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39">
+        <f>70/(B29^2*0.00000165)</f>
+        <v>1.4024542950162784E-4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="5">
+        <f>B39*1000000</f>
+        <v>140.24542950162783</v>
+      </c>
+      <c r="E39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <f>(0.08*B39*B37*1)/B34</f>
+        <v>1.5141527720895969</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40">
+        <f>B40*1000</f>
+        <v>1514.152772089597</v>
+      </c>
+      <c r="E40" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <f>(B7/(B8*B29))*((B17+B19)/(B17*B19))</f>
+        <v>1.5865779912246515E-10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="5">
+        <f>B44*1000000000000</f>
+        <v>158.65779912246515</v>
+      </c>
+      <c r="E44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47">
+        <f>1.2*B10</f>
+        <v>28.799999999999997</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" s="4">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="4">
+        <v>150</v>
+      </c>
+      <c r="C52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="4">
+        <v>30</v>
+      </c>
+      <c r="C53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54">
+        <f>B11^2*B49*B24</f>
+        <v>0.56470588235294128</v>
+      </c>
+      <c r="C54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f>0.5*B9*B11*0.0000000015*B29*(8.5/(B50-B51)+6.8/B51)</f>
+        <v>0.43349999999999994</v>
+      </c>
+      <c r="C55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56">
+        <f>B54+B55</f>
+        <v>0.99820588235294117</v>
+      </c>
+      <c r="C56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57">
+        <f>B52/B53</f>
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" s="4">
+        <f>B49</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" s="4">
+        <f>B50</f>
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" s="4">
+        <f>B51</f>
+        <v>1.6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" s="4">
+        <f>B52</f>
+        <v>150</v>
+      </c>
+      <c r="C62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" s="4">
+        <f>B53</f>
+        <v>30</v>
+      </c>
+      <c r="C63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64">
+        <f>B11^2*B59*(1-B24)</f>
+        <v>0.23529411764705879</v>
+      </c>
+      <c r="C64" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68">
+        <f>D14*B9</f>
+        <v>0.85000000000000009</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69">
+        <f>(B11*B24*(1-B24))/(B29*B68)</f>
+        <v>4.4409081657198891E-6</v>
+      </c>
+      <c r="C69" t="s">
+        <v>43</v>
+      </c>
+      <c r="D69" s="5">
+        <f>B69*1000000</f>
+        <v>4.4409081657198888</v>
+      </c>
+      <c r="E69" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72">
+        <v>0.6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="3">
+        <v>7.7000000000000008E-6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73">
+        <f>B73*1000000</f>
+        <v>7.7000000000000011</v>
+      </c>
+      <c r="E73" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74">
+        <f>-(B73*B13)/B72</f>
+        <v>-6.4166666666666691E-11</v>
+      </c>
+      <c r="C74" t="s">
+        <v>43</v>
+      </c>
+      <c r="D74">
+        <f>B74*1000000</f>
+        <v>-6.416666666666669E-5</v>
+      </c>
+      <c r="E74" t="s">
+        <v>36</v>
+      </c>
+      <c r="F74" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="lessThan">
+      <formula>$E$28</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
+      <formula>$F$28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
+      <formula>$G$18</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThan">
       <formula>$H$18</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1616,9 +3566,9 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" xr:uid="{E45BFA85-D7EA-4DEE-928D-EE60C8A55F03}"/>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{9DC082BC-1C68-412B-8D3E-87B60DE826D2}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 3.3V buck board
</commit_message>
<xml_diff>
--- a/doc/LM3150MHX Calculator.xlsx
+++ b/doc/LM3150MHX Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DCDC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7208DA5-29C5-4DC1-8B34-324C95A8E329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6764DC2F-2A2C-4066-A5C3-C7A5E60A6A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="530" yWindow="0" windowWidth="17320" windowHeight="19950" activeTab="1" xr2:uid="{C17DE87D-D3A8-4F0B-998C-A262C791429E}"/>
+    <workbookView xWindow="530" yWindow="0" windowWidth="17320" windowHeight="19950" activeTab="2" xr2:uid="{C17DE87D-D3A8-4F0B-998C-A262C791429E}"/>
   </bookViews>
   <sheets>
     <sheet name="5V" sheetId="1" r:id="rId1"/>
@@ -1013,7 +1013,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1867,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDCA830-8D2C-4258-99A0-6269838FD908}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1922,7 +1922,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="B25">
         <f>B7/B8</f>
-        <v>0.54999999999999993</v>
+        <v>0.65999999999999992</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -2140,14 +2140,14 @@
       </c>
       <c r="B27">
         <f>(1-B25)/B26</f>
-        <v>4.3636363636363641E-7</v>
+        <v>3.296969696969698E-7</v>
       </c>
       <c r="C27" t="s">
         <v>40</v>
       </c>
       <c r="D27">
         <f>B27*10000000</f>
-        <v>4.3636363636363642</v>
+        <v>3.2969696969696978</v>
       </c>
       <c r="E27" t="s">
         <v>18</v>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="B28">
         <f>(1-B25)/(B27+0.0000002)</f>
-        <v>707142.85714285716</v>
+        <v>641876.43020594981</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
@@ -2169,11 +2169,11 @@
       </c>
       <c r="E28">
         <f>B28-B28*D28</f>
-        <v>636428.57142857148</v>
+        <v>577688.78718535486</v>
       </c>
       <c r="F28">
         <f>B28+B28*D28</f>
-        <v>777857.14285714284</v>
+        <v>706064.07322654477</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -2363,14 +2363,14 @@
       </c>
       <c r="B44">
         <f>(B7/(B8*B29))*((B17+B19)/(B17*B19))</f>
-        <v>9.2778727523634948E-11</v>
+        <v>1.1133447302836192E-10</v>
       </c>
       <c r="C44" t="s">
         <v>43</v>
       </c>
       <c r="D44" s="5">
         <f>B44*1000000000000</f>
-        <v>92.778727523634942</v>
+        <v>111.33447302836193</v>
       </c>
       <c r="E44" t="s">
         <v>47</v>
@@ -2722,8 +2722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18A6C88-0247-4D30-92B5-0F853FB0062C}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2799,7 +2799,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="4">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -2956,7 +2956,7 @@
       </c>
       <c r="B23">
         <f>B7/B10</f>
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -2983,7 +2983,7 @@
       </c>
       <c r="B26">
         <f>B23/(0.0000002)</f>
-        <v>2500000</v>
+        <v>1875000</v>
       </c>
       <c r="C26" t="s">
         <v>39</v>
@@ -2995,14 +2995,14 @@
       </c>
       <c r="B27">
         <f>(1-B25)/B26</f>
-        <v>5.7142857142857164E-8</v>
+        <v>7.6190476190476219E-8</v>
       </c>
       <c r="C27" t="s">
         <v>40</v>
       </c>
       <c r="D27">
         <f>B27*10000000</f>
-        <v>0.57142857142857162</v>
+        <v>0.7619047619047622</v>
       </c>
       <c r="E27" t="s">
         <v>18</v>
@@ -3014,7 +3014,7 @@
       </c>
       <c r="B28">
         <f>(1-B25)/(B27+0.0000002)</f>
-        <v>555555.55555555574</v>
+        <v>517241.37931034499</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
@@ -3024,11 +3024,11 @@
       </c>
       <c r="E28">
         <f>B28-B28*D28</f>
-        <v>500000.00000000017</v>
+        <v>465517.24137931049</v>
       </c>
       <c r="F28">
         <f>B28+B28*D28</f>
-        <v>611111.11111111136</v>
+        <v>568965.51724137948</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -3098,14 +3098,14 @@
       </c>
       <c r="B34">
         <f>(B10-B7)*(B7/B10)*(1/B29)</f>
-        <v>1.0909090909090909E-5</v>
+        <v>1.3636363636363635E-5</v>
       </c>
       <c r="C34" t="s">
         <v>42</v>
       </c>
       <c r="D34">
         <f>B34*1000000</f>
-        <v>10.909090909090908</v>
+        <v>13.636363636363635</v>
       </c>
       <c r="E34" t="s">
         <v>31</v>
@@ -3183,14 +3183,14 @@
       </c>
       <c r="B40">
         <f>(0.08*B39*B37*1)/B34</f>
-        <v>1.5141527720895969</v>
+        <v>1.2113222176716776</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40">
         <f>B40*1000</f>
-        <v>1514.152772089597</v>
+        <v>1211.3222176716777</v>
       </c>
       <c r="E40" t="s">
         <v>51</v>
@@ -3242,7 +3242,7 @@
       </c>
       <c r="B47">
         <f>1.2*B10</f>
-        <v>28.799999999999997</v>
+        <v>38.4</v>
       </c>
       <c r="C47" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Fixed few values on 3.3V schematics. Generated CAM files.
</commit_message>
<xml_diff>
--- a/doc/LM3150MHX Calculator.xlsx
+++ b/doc/LM3150MHX Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DCDC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6764DC2F-2A2C-4066-A5C3-C7A5E60A6A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0C7247-1AEB-4CCB-84B4-F5F31A22F81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="530" yWindow="0" windowWidth="17320" windowHeight="19950" activeTab="2" xr2:uid="{C17DE87D-D3A8-4F0B-998C-A262C791429E}"/>
   </bookViews>
@@ -1868,7 +1868,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2181,14 +2181,14 @@
         <v>27</v>
       </c>
       <c r="B29" s="4">
-        <v>700000</v>
+        <v>600000</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
       </c>
       <c r="D29">
         <f>B29/1000</f>
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -2219,14 +2219,14 @@
       </c>
       <c r="B31">
         <f>((B7*B9)-B7)/(B9*0.0000000001*B29)+(B30)</f>
-        <v>38936.28571428571</v>
+        <v>46138.666666666657</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
       </c>
       <c r="D31" s="5">
         <f>B31/1000</f>
-        <v>38.93628571428571</v>
+        <v>46.138666666666659</v>
       </c>
       <c r="E31" t="s">
         <v>23</v>
@@ -2243,14 +2243,14 @@
       </c>
       <c r="B34">
         <f>(B10-B7)*(B7/B10)*(1/B29)</f>
-        <v>3.7419642857142854E-6</v>
+        <v>4.3656249999999994E-6</v>
       </c>
       <c r="C34" t="s">
         <v>42</v>
       </c>
       <c r="D34">
         <f>B34*1000000</f>
-        <v>3.7419642857142854</v>
+        <v>4.3656249999999996</v>
       </c>
       <c r="E34" t="s">
         <v>31</v>
@@ -2290,14 +2290,14 @@
       </c>
       <c r="B38">
         <f>(B7/B9)/B29</f>
-        <v>3.9285714285714281E-7</v>
+        <v>4.5833333333333327E-7</v>
       </c>
       <c r="C38" t="s">
         <v>40</v>
       </c>
       <c r="D38">
         <f>B38*1000000000</f>
-        <v>392.85714285714283</v>
+        <v>458.33333333333326</v>
       </c>
       <c r="E38" t="s">
         <v>24</v>
@@ -2309,14 +2309,14 @@
       </c>
       <c r="B39">
         <f>70/(B29^2*0.00000165)</f>
-        <v>8.658008658008658E-5</v>
+        <v>1.1784511784511784E-4</v>
       </c>
       <c r="C39" t="s">
         <v>43</v>
       </c>
       <c r="D39" s="5">
         <f>B39*1000000</f>
-        <v>86.580086580086586</v>
+        <v>117.84511784511784</v>
       </c>
       <c r="E39" t="s">
         <v>36</v>
@@ -2328,14 +2328,14 @@
       </c>
       <c r="B40">
         <f>(0.08*B39*B37*1)/B34</f>
-        <v>1.9236242456243144</v>
+        <v>2.2442282865617003</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40">
         <f>B40*1000</f>
-        <v>1923.6242456243144</v>
+        <v>2244.2282865617003</v>
       </c>
       <c r="E40" t="s">
         <v>51</v>
@@ -2363,14 +2363,14 @@
       </c>
       <c r="B44">
         <f>(B7/(B8*B29))*((B17+B19)/(B17*B19))</f>
-        <v>1.1133447302836192E-10</v>
+        <v>1.2989021853308889E-10</v>
       </c>
       <c r="C44" t="s">
         <v>43</v>
       </c>
       <c r="D44" s="5">
         <f>B44*1000000000000</f>
-        <v>111.33447302836193</v>
+        <v>129.8902185330889</v>
       </c>
       <c r="E44" t="s">
         <v>47</v>
@@ -2474,7 +2474,7 @@
       </c>
       <c r="B55">
         <f>0.5*B9*B11*0.0000000015*B29*(8.5/(B50-B51)+6.8/B51)</f>
-        <v>0.38945454545454544</v>
+        <v>0.33381818181818179</v>
       </c>
       <c r="C55" t="s">
         <v>53</v>
@@ -2486,7 +2486,7 @@
       </c>
       <c r="B56">
         <f>B54+B55</f>
-        <v>0.60945454545454547</v>
+        <v>0.55381818181818177</v>
       </c>
       <c r="C56" t="s">
         <v>53</v>
@@ -2609,14 +2609,14 @@
       </c>
       <c r="B69">
         <f>(B11*B24*(1-B24))/(B29*B68)</f>
-        <v>4.7470238095238085E-6</v>
+        <v>5.5381944444444436E-6</v>
       </c>
       <c r="C69" t="s">
         <v>43</v>
       </c>
       <c r="D69" s="5">
         <f>B69*1000000</f>
-        <v>4.7470238095238084</v>
+        <v>5.5381944444444438</v>
       </c>
       <c r="E69" t="s">
         <v>36</v>
@@ -2723,7 +2723,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2871,15 +2871,15 @@
         <v>22</v>
       </c>
       <c r="B17" s="4">
-        <f>10000+330</f>
-        <v>10330</v>
+        <f>10000+470</f>
+        <v>10470</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17">
         <f>B17/1000</f>
-        <v>10.33</v>
+        <v>10.47</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
@@ -2891,14 +2891,14 @@
       </c>
       <c r="B18">
         <f>B17*(B7/B4-1)</f>
-        <v>196270</v>
+        <v>198930</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D18">
         <f>B18/1000</f>
-        <v>196.27</v>
+        <v>198.93</v>
       </c>
       <c r="E18" t="s">
         <v>23</v>
@@ -2908,11 +2908,11 @@
       </c>
       <c r="G18">
         <f>B18-B18*F18</f>
-        <v>192344.6</v>
+        <v>194951.4</v>
       </c>
       <c r="H18">
         <f>B18+B18*F18</f>
-        <v>200195.4</v>
+        <v>202908.6</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="B20" s="5">
         <f>(B19/B17+1)*B4</f>
-        <v>12.216650532429815</v>
+        <v>12.061318051575929</v>
       </c>
       <c r="C20" t="s">
         <v>13</v>
@@ -3036,14 +3036,14 @@
         <v>27</v>
       </c>
       <c r="B29" s="4">
-        <v>550000</v>
+        <v>500000</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
       </c>
       <c r="D29">
         <f>B29/1000</f>
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -3074,14 +3074,14 @@
       </c>
       <c r="B31">
         <f>((B7*B9)-B7)/(B9*0.0000000001*B29)+(B30)</f>
-        <v>198259.5935828877</v>
+        <v>218794.35294117645</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
       </c>
       <c r="D31" s="5">
         <f>B31/1000</f>
-        <v>198.2595935828877</v>
+        <v>218.79435294117644</v>
       </c>
       <c r="E31" t="s">
         <v>23</v>
@@ -3098,14 +3098,14 @@
       </c>
       <c r="B34">
         <f>(B10-B7)*(B7/B10)*(1/B29)</f>
-        <v>1.3636363636363635E-5</v>
+        <v>1.4999999999999999E-5</v>
       </c>
       <c r="C34" t="s">
         <v>42</v>
       </c>
       <c r="D34">
         <f>B34*1000000</f>
-        <v>13.636363636363635</v>
+        <v>14.999999999999998</v>
       </c>
       <c r="E34" t="s">
         <v>31</v>
@@ -3145,14 +3145,14 @@
       </c>
       <c r="B38">
         <f>(B7/B9)/B29</f>
-        <v>1.2834224598930481E-6</v>
+        <v>1.4117647058823531E-6</v>
       </c>
       <c r="C38" t="s">
         <v>40</v>
       </c>
       <c r="D38">
         <f>B38*1000000000</f>
-        <v>1283.4224598930482</v>
+        <v>1411.7647058823532</v>
       </c>
       <c r="E38" t="s">
         <v>24</v>
@@ -3164,14 +3164,14 @@
       </c>
       <c r="B39">
         <f>70/(B29^2*0.00000165)</f>
-        <v>1.4024542950162784E-4</v>
+        <v>1.6969696969696969E-4</v>
       </c>
       <c r="C39" t="s">
         <v>43</v>
       </c>
       <c r="D39" s="5">
         <f>B39*1000000</f>
-        <v>140.24542950162783</v>
+        <v>169.69696969696969</v>
       </c>
       <c r="E39" t="s">
         <v>36</v>
@@ -3183,14 +3183,14 @@
       </c>
       <c r="B40">
         <f>(0.08*B39*B37*1)/B34</f>
-        <v>1.2113222176716776</v>
+        <v>1.3324544394388456</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40">
         <f>B40*1000</f>
-        <v>1211.3222176716777</v>
+        <v>1332.4544394388456</v>
       </c>
       <c r="E40" t="s">
         <v>51</v>
@@ -3218,14 +3218,14 @@
       </c>
       <c r="B44">
         <f>(B7/(B8*B29))*((B17+B19)/(B17*B19))</f>
-        <v>1.5865779912246515E-10</v>
+        <v>1.7230454359394187E-10</v>
       </c>
       <c r="C44" t="s">
         <v>43</v>
       </c>
       <c r="D44" s="5">
         <f>B44*1000000000000</f>
-        <v>158.65779912246515</v>
+        <v>172.30454359394187</v>
       </c>
       <c r="E44" t="s">
         <v>47</v>
@@ -3329,7 +3329,7 @@
       </c>
       <c r="B55">
         <f>0.5*B9*B11*0.0000000015*B29*(8.5/(B50-B51)+6.8/B51)</f>
-        <v>0.43349999999999994</v>
+        <v>0.3940909090909091</v>
       </c>
       <c r="C55" t="s">
         <v>53</v>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="B56">
         <f>B54+B55</f>
-        <v>0.99820588235294117</v>
+        <v>0.95879679144385044</v>
       </c>
       <c r="C56" t="s">
         <v>53</v>
@@ -3464,14 +3464,14 @@
       </c>
       <c r="B69">
         <f>(B11*B24*(1-B24))/(B29*B68)</f>
-        <v>4.4409081657198891E-6</v>
+        <v>4.884998982291878E-6</v>
       </c>
       <c r="C69" t="s">
         <v>43</v>
       </c>
       <c r="D69" s="5">
         <f>B69*1000000</f>
-        <v>4.4409081657198888</v>
+        <v>4.8849989822918776</v>
       </c>
       <c r="E69" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Added 12V buck converter. Generated CAM files.
</commit_message>
<xml_diff>
--- a/doc/LM3150MHX Calculator.xlsx
+++ b/doc/LM3150MHX Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DCDC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0C7247-1AEB-4CCB-84B4-F5F31A22F81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F014CAB-800C-44D7-B722-A4BCDC3DF142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="530" yWindow="0" windowWidth="17320" windowHeight="19950" activeTab="2" xr2:uid="{C17DE87D-D3A8-4F0B-998C-A262C791429E}"/>
+    <workbookView xWindow="530" yWindow="0" windowWidth="17320" windowHeight="19950" xr2:uid="{C17DE87D-D3A8-4F0B-998C-A262C791429E}"/>
   </bookViews>
   <sheets>
     <sheet name="5V" sheetId="1" r:id="rId1"/>
@@ -1012,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C0D372-FD9A-401D-80C0-F303A26CDA15}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1868,7 +1868,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2722,8 +2722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18A6C88-0247-4D30-92B5-0F853FB0062C}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3523,8 +3523,8 @@
         <v>43</v>
       </c>
       <c r="D74">
-        <f>B74*1000000</f>
-        <v>-6.416666666666669E-5</v>
+        <f>B74*100000000</f>
+        <v>-6.4166666666666695E-3</v>
       </c>
       <c r="E74" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Made new layout of DC-DC board. Improved XLS calculator. Generated CAM files. Generated BoM and PnP files. Generated PNG preview. Generated PDF schematics.
</commit_message>
<xml_diff>
--- a/doc/LM3150MHX Calculator.xlsx
+++ b/doc/LM3150MHX Calculator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DCDC\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DC-DC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F014CAB-800C-44D7-B722-A4BCDC3DF142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA155C81-F86E-43AB-9706-3CCC6AD80ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="530" yWindow="0" windowWidth="17320" windowHeight="19950" xr2:uid="{C17DE87D-D3A8-4F0B-998C-A262C791429E}"/>
   </bookViews>
@@ -1013,7 +1013,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,14 +1161,15 @@
         <v>22</v>
       </c>
       <c r="B17" s="4">
-        <v>10000</v>
+        <f>10000+100</f>
+        <v>10100</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17">
         <f>B17/1000</f>
-        <v>10</v>
+        <v>10.1</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
@@ -1180,14 +1181,14 @@
       </c>
       <c r="B18">
         <f>B17*(B7/B4-1)</f>
-        <v>73333.333333333343</v>
+        <v>74066.666666666672</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D18">
         <f>B18/1000</f>
-        <v>73.333333333333343</v>
+        <v>74.066666666666677</v>
       </c>
       <c r="E18" t="s">
         <v>23</v>
@@ -1197,11 +1198,11 @@
       </c>
       <c r="G18">
         <f>B18-B18*F18</f>
-        <v>71866.666666666672</v>
+        <v>72585.333333333343</v>
       </c>
       <c r="H18">
         <f>B18+B18*F18</f>
-        <v>74800.000000000015</v>
+        <v>75548</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1209,15 +1210,15 @@
         <v>4</v>
       </c>
       <c r="B19" s="4">
-        <f>68000+3000+3000</f>
-        <v>74000</v>
+        <f>75000</f>
+        <v>75000</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
       </c>
       <c r="D19">
         <f>B19/1000</f>
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E19" t="s">
         <v>23</v>
@@ -1229,7 +1230,7 @@
       </c>
       <c r="B20" s="5">
         <f>(B19/B17+1)*B4</f>
-        <v>5.04</v>
+        <v>5.0554455445544564</v>
       </c>
       <c r="C20" t="s">
         <v>13</v>
@@ -1508,14 +1509,14 @@
       </c>
       <c r="B44">
         <f>(B7/(B8*B29))*((B17+B19)/(B17*B19))</f>
-        <v>1.8918918918918919E-10</v>
+        <v>1.8723872387238723E-10</v>
       </c>
       <c r="C44" t="s">
         <v>43</v>
       </c>
       <c r="D44" s="5">
         <f>B44*1000000000000</f>
-        <v>189.18918918918919</v>
+        <v>187.23872387238723</v>
       </c>
       <c r="E44" t="s">
         <v>47</v>
@@ -1868,7 +1869,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2723,7 +2724,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Renamed 17V boards to 18V. No other changes are made.
</commit_message>
<xml_diff>
--- a/doc/LM3150MHX Calculator.xlsx
+++ b/doc/LM3150MHX Calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DC-DC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA155C81-F86E-43AB-9706-3CCC6AD80ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7D0F49-4A87-4984-8FA4-39337EF295A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="530" yWindow="0" windowWidth="17320" windowHeight="19950" xr2:uid="{C17DE87D-D3A8-4F0B-998C-A262C791429E}"/>
+    <workbookView xWindow="21020" yWindow="670" windowWidth="19550" windowHeight="19950" activeTab="2" xr2:uid="{C17DE87D-D3A8-4F0B-998C-A262C791429E}"/>
   </bookViews>
   <sheets>
     <sheet name="5V" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1012,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C0D372-FD9A-401D-80C0-F303A26CDA15}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2723,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18A6C88-0247-4D30-92B5-0F853FB0062C}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2789,7 +2796,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -2966,7 +2973,7 @@
       </c>
       <c r="B24">
         <f>B7/B9</f>
-        <v>0.70588235294117652</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -3056,14 +3063,14 @@
       </c>
       <c r="B30">
         <f>-((B9-1)*(B9*16.5+100))-1000</f>
-        <v>-7088</v>
+        <v>-7749</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
       </c>
       <c r="D30">
         <f>B30/1000</f>
-        <v>-7.0880000000000001</v>
+        <v>-7.7489999999999997</v>
       </c>
       <c r="E30" t="s">
         <v>23</v>
@@ -3075,14 +3082,14 @@
       </c>
       <c r="B31">
         <f>((B7*B9)-B7)/(B9*0.0000000001*B29)+(B30)</f>
-        <v>218794.35294117645</v>
+        <v>218917.66666666669</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
       </c>
       <c r="D31" s="5">
         <f>B31/1000</f>
-        <v>218.79435294117644</v>
+        <v>218.91766666666669</v>
       </c>
       <c r="E31" t="s">
         <v>23</v>
@@ -3123,7 +3130,7 @@
       </c>
       <c r="B37">
         <f>B9*0.3/12^(1/2)</f>
-        <v>1.4722431864335457</v>
+        <v>1.5588457268119895</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
@@ -3133,11 +3140,11 @@
       </c>
       <c r="E37">
         <f>B37-B37*D37</f>
-        <v>1.3986310271118685</v>
+        <v>1.4809034404713901</v>
       </c>
       <c r="F37">
         <f>B37+B37*D37</f>
-        <v>1.5458553457552229</v>
+        <v>1.6367880131525889</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -3146,14 +3153,14 @@
       </c>
       <c r="B38">
         <f>(B7/B9)/B29</f>
-        <v>1.4117647058823531E-6</v>
+        <v>1.3333333333333332E-6</v>
       </c>
       <c r="C38" t="s">
         <v>40</v>
       </c>
       <c r="D38">
         <f>B38*1000000000</f>
-        <v>1411.7647058823532</v>
+        <v>1333.3333333333333</v>
       </c>
       <c r="E38" t="s">
         <v>24</v>
@@ -3184,14 +3191,14 @@
       </c>
       <c r="B40">
         <f>(0.08*B39*B37*1)/B34</f>
-        <v>1.3324544394388456</v>
+        <v>1.4108341123470129</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40">
         <f>B40*1000</f>
-        <v>1332.4544394388456</v>
+        <v>1410.8341123470129</v>
       </c>
       <c r="E40" t="s">
         <v>51</v>
@@ -3318,7 +3325,7 @@
       </c>
       <c r="B54">
         <f>B11^2*B49*B24</f>
-        <v>0.56470588235294128</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="C54" t="s">
         <v>53</v>
@@ -3330,7 +3337,7 @@
       </c>
       <c r="B55">
         <f>0.5*B9*B11*0.0000000015*B29*(8.5/(B50-B51)+6.8/B51)</f>
-        <v>0.3940909090909091</v>
+        <v>0.4172727272727273</v>
       </c>
       <c r="C55" t="s">
         <v>53</v>
@@ -3342,7 +3349,7 @@
       </c>
       <c r="B56">
         <f>B54+B55</f>
-        <v>0.95879679144385044</v>
+        <v>0.95060606060606068</v>
       </c>
       <c r="C56" t="s">
         <v>53</v>
@@ -3431,7 +3438,7 @@
       </c>
       <c r="B64">
         <f>B11^2*B59*(1-B24)</f>
-        <v>0.23529411764705879</v>
+        <v>0.26666666666666672</v>
       </c>
       <c r="C64" t="s">
         <v>53</v>
@@ -3456,7 +3463,7 @@
       </c>
       <c r="B68">
         <f>D14*B9</f>
-        <v>0.85000000000000009</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -3465,14 +3472,14 @@
       </c>
       <c r="B69">
         <f>(B11*B24*(1-B24))/(B29*B68)</f>
-        <v>4.884998982291878E-6</v>
+        <v>4.9382716049382717E-6</v>
       </c>
       <c r="C69" t="s">
         <v>43</v>
       </c>
       <c r="D69" s="5">
         <f>B69*1000000</f>
-        <v>4.8849989822918776</v>
+        <v>4.9382716049382713</v>
       </c>
       <c r="E69" t="s">
         <v>36</v>

</xml_diff>